<commit_message>
CH-0160 zu EAD_v1.xlsx korrigieren
git-svn-id: svn://localhost/DI-Extractor@52 38a3ecd8-5b25-7645-a312-2ec681589999
</commit_message>
<xml_diff>
--- a/app/eCH-0160 zu EAD_v1.xlsx
+++ b/app/eCH-0160 zu EAD_v1.xlsx
@@ -7,11 +7,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="24120" windowHeight="12825" tabRatio="141"/>
   </bookViews>
   <sheets>
-    <sheet name="eCH-0160 zu xIsadg" sheetId="1" r:id="rId1"/>
+    <sheet name="eCH-0160 zu EAD" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'eCH-0160 zu xIsadg'!$A$1:$J$42</definedName>
-    <definedName name="Print_Area" localSheetId="0">'eCH-0160 zu xIsadg'!$A$1:$J$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'eCH-0160 zu EAD'!$A$1:$J$42</definedName>
+    <definedName name="Print_Area" localSheetId="0">'eCH-0160 zu EAD'!$A$1:$J$42</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -750,9 +750,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -767,27 +788,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1161,8 +1161,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J38" sqref="A1:J38"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -1212,11 +1212,11 @@
       <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:11" s="3" customFormat="1" ht="25.5">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
       <c r="D2" s="35" t="s">
         <v>10</v>
       </c>
@@ -1233,7 +1233,7 @@
       <c r="I2" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="44" t="s">
+      <c r="J2" s="37" t="s">
         <v>15</v>
       </c>
       <c r="K2" s="15"/>
@@ -1254,7 +1254,7 @@
       <c r="I3" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="45" t="s">
+      <c r="J3" s="38" t="s">
         <v>19</v>
       </c>
       <c r="K3" s="15"/>
@@ -1275,7 +1275,7 @@
       <c r="I4" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="45" t="s">
+      <c r="J4" s="38" t="s">
         <v>23</v>
       </c>
       <c r="K4" s="15"/>
@@ -1296,7 +1296,7 @@
       <c r="I5" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="J5" s="45" t="s">
+      <c r="J5" s="38" t="s">
         <v>27</v>
       </c>
       <c r="K5" s="15"/>
@@ -1325,7 +1325,7 @@
       <c r="I6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="46" t="s">
+      <c r="J6" s="39" t="s">
         <v>35</v>
       </c>
       <c r="K6" s="15"/>
@@ -1350,7 +1350,7 @@
       <c r="I7" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="45" t="s">
+      <c r="J7" s="38" t="s">
         <v>41</v>
       </c>
       <c r="K7" s="16"/>
@@ -1367,7 +1367,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="4"/>
       <c r="I8" s="36"/>
-      <c r="J8" s="45" t="s">
+      <c r="J8" s="38" t="s">
         <v>43</v>
       </c>
       <c r="K8" s="15"/>
@@ -1384,7 +1384,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="4"/>
       <c r="I9" s="36"/>
-      <c r="J9" s="45"/>
+      <c r="J9" s="38"/>
       <c r="K9" s="16"/>
     </row>
     <row r="10" spans="1:11" s="3" customFormat="1">
@@ -1399,7 +1399,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="4"/>
       <c r="I10" s="36"/>
-      <c r="J10" s="47" t="s">
+      <c r="J10" s="40" t="s">
         <v>46</v>
       </c>
       <c r="K10" s="15"/>
@@ -1428,7 +1428,7 @@
       <c r="I11" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="J11" s="46" t="s">
+      <c r="J11" s="39" t="s">
         <v>52</v>
       </c>
       <c r="K11" s="15"/>
@@ -1445,7 +1445,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="4"/>
       <c r="I12" s="36"/>
-      <c r="J12" s="45" t="s">
+      <c r="J12" s="38" t="s">
         <v>54</v>
       </c>
       <c r="K12" s="16"/>
@@ -1466,7 +1466,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="4"/>
       <c r="I13" s="36"/>
-      <c r="J13" s="47" t="s">
+      <c r="J13" s="40" t="s">
         <v>46</v>
       </c>
       <c r="K13" s="15"/>
@@ -1489,7 +1489,7 @@
       <c r="I14" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="J14" s="45" t="s">
+      <c r="J14" s="38" t="s">
         <v>59</v>
       </c>
       <c r="K14" s="15"/>
@@ -1512,7 +1512,7 @@
       <c r="I15" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="J15" s="45" t="s">
+      <c r="J15" s="38" t="s">
         <v>64</v>
       </c>
       <c r="K15" s="16"/>
@@ -1529,7 +1529,7 @@
       <c r="G16" s="2"/>
       <c r="H16" s="4"/>
       <c r="I16" s="36"/>
-      <c r="J16" s="47" t="s">
+      <c r="J16" s="40" t="s">
         <v>66</v>
       </c>
       <c r="K16" s="15"/>
@@ -1550,7 +1550,7 @@
       <c r="I17" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="J17" s="45" t="s">
+      <c r="J17" s="38" t="s">
         <v>43</v>
       </c>
       <c r="K17" s="15"/>
@@ -1571,7 +1571,7 @@
       <c r="G18" s="2"/>
       <c r="H18" s="4"/>
       <c r="I18" s="36"/>
-      <c r="J18" s="45" t="s">
+      <c r="J18" s="38" t="s">
         <v>19</v>
       </c>
       <c r="K18" s="16"/>
@@ -1590,7 +1590,7 @@
       <c r="G19" s="2"/>
       <c r="H19" s="4"/>
       <c r="I19" s="36"/>
-      <c r="J19" s="45" t="s">
+      <c r="J19" s="38" t="s">
         <v>74</v>
       </c>
       <c r="K19" s="16"/>
@@ -1607,7 +1607,7 @@
       <c r="G20" s="2"/>
       <c r="H20" s="4"/>
       <c r="I20" s="36"/>
-      <c r="J20" s="45" t="s">
+      <c r="J20" s="38" t="s">
         <v>76</v>
       </c>
       <c r="K20" s="16"/>
@@ -1636,7 +1636,7 @@
       <c r="I21" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="J21" s="45" t="s">
+      <c r="J21" s="38" t="s">
         <v>82</v>
       </c>
       <c r="K21" s="15"/>
@@ -1653,7 +1653,7 @@
       <c r="G22" s="2"/>
       <c r="H22" s="4"/>
       <c r="I22" s="36"/>
-      <c r="J22" s="45" t="s">
+      <c r="J22" s="38" t="s">
         <v>84</v>
       </c>
       <c r="K22" s="15"/>
@@ -1670,7 +1670,7 @@
       <c r="G23" s="2"/>
       <c r="H23" s="4"/>
       <c r="I23" s="36"/>
-      <c r="J23" s="45" t="s">
+      <c r="J23" s="38" t="s">
         <v>86</v>
       </c>
       <c r="K23" s="15"/>
@@ -1685,13 +1685,13 @@
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="42" t="s">
+      <c r="H24" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="I24" s="43" t="s">
+      <c r="I24" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="J24" s="37" t="s">
+      <c r="J24" s="43" t="s">
         <v>90</v>
       </c>
       <c r="K24" s="15"/>
@@ -1710,9 +1710,9 @@
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="48"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="44"/>
       <c r="K25" s="15"/>
     </row>
     <row r="26" spans="1:11" s="3" customFormat="1">
@@ -1729,9 +1729,9 @@
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="48"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="44"/>
       <c r="K26" s="15"/>
     </row>
     <row r="27" spans="1:11" s="3" customFormat="1">
@@ -1746,9 +1746,9 @@
       </c>
       <c r="F27" s="4"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="48"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="44"/>
       <c r="K27" s="15"/>
     </row>
     <row r="28" spans="1:11" s="3" customFormat="1">
@@ -1765,9 +1765,9 @@
         <v>94</v>
       </c>
       <c r="G28" s="2"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="48"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="44"/>
       <c r="K28" s="15"/>
     </row>
     <row r="29" spans="1:11" s="3" customFormat="1">
@@ -1784,9 +1784,9 @@
         <v>95</v>
       </c>
       <c r="G29" s="2"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="48"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="44"/>
       <c r="K29" s="15"/>
     </row>
     <row r="30" spans="1:11" s="3" customFormat="1">
@@ -1803,9 +1803,9 @@
         <v>96</v>
       </c>
       <c r="G30" s="2"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="48"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="44"/>
       <c r="K30" s="15"/>
     </row>
     <row r="31" spans="1:11" s="3" customFormat="1">
@@ -1822,9 +1822,9 @@
         <v>97</v>
       </c>
       <c r="G31" s="2"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="48"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="44"/>
       <c r="K31" s="15"/>
     </row>
     <row r="32" spans="1:11" s="3" customFormat="1">
@@ -1841,9 +1841,9 @@
         <v>98</v>
       </c>
       <c r="G32" s="2"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="48"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="44"/>
       <c r="K32" s="15"/>
     </row>
     <row r="33" spans="1:11" s="3" customFormat="1">
@@ -1858,7 +1858,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="4"/>
       <c r="I33" s="36"/>
-      <c r="J33" s="45"/>
+      <c r="J33" s="38"/>
       <c r="K33" s="15"/>
     </row>
     <row r="34" spans="1:11" s="3" customFormat="1">
@@ -1885,7 +1885,7 @@
       <c r="I34" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="J34" s="47" t="s">
+      <c r="J34" s="40" t="s">
         <v>103</v>
       </c>
       <c r="K34" s="15"/>
@@ -1904,7 +1904,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="4"/>
       <c r="I35" s="36"/>
-      <c r="J35" s="45" t="s">
+      <c r="J35" s="38" t="s">
         <v>105</v>
       </c>
       <c r="K35" s="15"/>
@@ -1929,7 +1929,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="4"/>
       <c r="I36" s="36"/>
-      <c r="J36" s="45" t="s">
+      <c r="J36" s="38" t="s">
         <v>107</v>
       </c>
       <c r="K36" s="15"/>
@@ -1946,7 +1946,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="4"/>
       <c r="I37" s="36"/>
-      <c r="J37" s="45"/>
+      <c r="J37" s="38"/>
       <c r="K37" s="15"/>
     </row>
     <row r="38" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
@@ -1965,7 +1965,7 @@
       <c r="I38" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="J38" s="49" t="s">
+      <c r="J38" s="41" t="s">
         <v>112</v>
       </c>
       <c r="K38" s="15"/>
@@ -1983,39 +1983,39 @@
       <c r="J39" s="18"/>
     </row>
     <row r="40" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A40" s="38" t="s">
+      <c r="A40" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="B40" s="38"/>
+      <c r="B40" s="45"/>
       <c r="C40" s="12"/>
       <c r="J40" s="9"/>
     </row>
     <row r="41" spans="1:11" s="3" customFormat="1" ht="12" customHeight="1">
-      <c r="A41" s="38" t="s">
+      <c r="A41" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="B41" s="38"/>
+      <c r="B41" s="45"/>
       <c r="C41" s="13"/>
       <c r="J41" s="9"/>
     </row>
     <row r="42" spans="1:11" s="3" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="46"/>
       <c r="C42" s="14"/>
       <c r="J42" s="9"/>
       <c r="K42" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="H24:H32"/>
     <mergeCell ref="I24:I32"/>
     <mergeCell ref="J24:J32"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.15748031496062992" top="1.0236220472440944" bottom="0.43307086614173229" header="0.51181102362204722" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="59" orientation="landscape" useFirstPageNumber="1" r:id="rId1"/>

</xml_diff>